<commit_message>
add [CoordinateMgr class] getCoordinateDataCSV -> read Coordinate setup from csv.
</commit_message>
<xml_diff>
--- a/CoordinateData_Robot1_01.xlsx
+++ b/CoordinateData_Robot1_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waltz\Documents\CppProjects\GitManagements\QuantumCoreRobotReNew_0104\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6447CC96-9950-4000-BA3E-46685D20E89B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C87FB26B-325F-46B9-BA4D-E21E676A5DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="2280" windowWidth="29040" windowHeight="15840" xr2:uid="{4A88D659-4C13-44B6-A2BE-41980A9F7671}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t>id</t>
     <phoneticPr fontId="1"/>
@@ -136,6 +136,30 @@
   </si>
   <si>
     <t>RA03</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Show</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Coordinate</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>on</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>on/off</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>size</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>length</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -963,11 +987,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70A82EBB-6C3C-46D3-B3DF-77C251B3AEE0}">
-  <dimension ref="A1:AD104"/>
+  <dimension ref="A1:AG104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y15" sqref="Y15"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:AD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -978,10 +1002,11 @@
     <col min="4" max="4" width="12.5" style="1" customWidth="1"/>
     <col min="5" max="7" width="4.25" style="1" customWidth="1"/>
     <col min="8" max="29" width="4.375" style="1" customWidth="1"/>
-    <col min="30" max="30" width="30.875" style="1" customWidth="1"/>
+    <col min="30" max="32" width="7.125" style="1" customWidth="1"/>
+    <col min="33" max="33" width="30.875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
@@ -1031,11 +1056,16 @@
       </c>
       <c r="AB1" s="19"/>
       <c r="AC1" s="20"/>
-      <c r="AD1" s="40" t="s">
+      <c r="AD1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE1" s="7"/>
+      <c r="AF1" s="10"/>
+      <c r="AG1" s="40" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A2" s="21" t="s">
         <v>0</v>
       </c>
@@ -1077,9 +1107,14 @@
       <c r="AA2" s="18"/>
       <c r="AB2" s="19"/>
       <c r="AC2" s="20"/>
-      <c r="AD2" s="40"/>
-    </row>
-    <row r="3" spans="1:30" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="AD2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="40"/>
+    </row>
+    <row r="3" spans="1:33" ht="19.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="29"/>
       <c r="B3" s="30"/>
       <c r="C3" s="31"/>
@@ -1157,9 +1192,18 @@
       <c r="AC3" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="AD3" s="32"/>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD3" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE3" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF3" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG3" s="32"/>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A4" s="4">
         <v>0</v>
       </c>
@@ -1243,11 +1287,20 @@
       <c r="AC4" s="28">
         <v>1</v>
       </c>
-      <c r="AD4" s="28" t="s">
+      <c r="AD4" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE4" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="AF4" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="AG4" s="28" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>200</v>
       </c>
@@ -1333,11 +1386,20 @@
       <c r="AC5" s="28">
         <v>1</v>
       </c>
-      <c r="AD5" s="12" t="s">
+      <c r="AD5" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE5" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="AF5" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="AG5" s="12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>201</v>
       </c>
@@ -1423,11 +1485,20 @@
       <c r="AC6" s="28">
         <v>1</v>
       </c>
-      <c r="AD6" s="12" t="s">
+      <c r="AD6" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE6" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="AF6" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="AG6" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>202</v>
       </c>
@@ -1513,11 +1584,20 @@
       <c r="AC7" s="28">
         <v>1</v>
       </c>
-      <c r="AD7" s="12" t="s">
+      <c r="AD7" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE7" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="AF7" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="AG7" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A8" s="3"/>
       <c r="B8" s="8"/>
       <c r="C8" s="11"/>
@@ -1547,9 +1627,12 @@
       <c r="AA8" s="11"/>
       <c r="AB8" s="3"/>
       <c r="AC8" s="12"/>
-      <c r="AD8" s="12"/>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD8" s="11"/>
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="12"/>
+      <c r="AG8" s="12"/>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A9" s="3"/>
       <c r="B9" s="8"/>
       <c r="C9" s="11"/>
@@ -1579,9 +1662,12 @@
       <c r="AA9" s="11"/>
       <c r="AB9" s="3"/>
       <c r="AC9" s="12"/>
-      <c r="AD9" s="12"/>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD9" s="11"/>
+      <c r="AE9" s="3"/>
+      <c r="AF9" s="12"/>
+      <c r="AG9" s="12"/>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A10" s="3"/>
       <c r="B10" s="8"/>
       <c r="C10" s="11"/>
@@ -1611,9 +1697,12 @@
       <c r="AA10" s="11"/>
       <c r="AB10" s="3"/>
       <c r="AC10" s="12"/>
-      <c r="AD10" s="12"/>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD10" s="11"/>
+      <c r="AE10" s="3"/>
+      <c r="AF10" s="12"/>
+      <c r="AG10" s="12"/>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A11" s="3"/>
       <c r="B11" s="8"/>
       <c r="C11" s="11"/>
@@ -1643,9 +1732,12 @@
       <c r="AA11" s="11"/>
       <c r="AB11" s="3"/>
       <c r="AC11" s="12"/>
-      <c r="AD11" s="12"/>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD11" s="11"/>
+      <c r="AE11" s="3"/>
+      <c r="AF11" s="12"/>
+      <c r="AG11" s="12"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A12" s="3"/>
       <c r="B12" s="8"/>
       <c r="C12" s="11"/>
@@ -1675,9 +1767,12 @@
       <c r="AA12" s="11"/>
       <c r="AB12" s="3"/>
       <c r="AC12" s="12"/>
-      <c r="AD12" s="12"/>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD12" s="11"/>
+      <c r="AE12" s="3"/>
+      <c r="AF12" s="12"/>
+      <c r="AG12" s="12"/>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A13" s="3"/>
       <c r="B13" s="8"/>
       <c r="C13" s="11"/>
@@ -1707,9 +1802,12 @@
       <c r="AA13" s="11"/>
       <c r="AB13" s="3"/>
       <c r="AC13" s="12"/>
-      <c r="AD13" s="12"/>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD13" s="11"/>
+      <c r="AE13" s="3"/>
+      <c r="AF13" s="12"/>
+      <c r="AG13" s="12"/>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A14" s="3"/>
       <c r="B14" s="8"/>
       <c r="C14" s="11"/>
@@ -1739,9 +1837,12 @@
       <c r="AA14" s="11"/>
       <c r="AB14" s="3"/>
       <c r="AC14" s="12"/>
-      <c r="AD14" s="12"/>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD14" s="11"/>
+      <c r="AE14" s="3"/>
+      <c r="AF14" s="12"/>
+      <c r="AG14" s="12"/>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A15" s="3"/>
       <c r="B15" s="8"/>
       <c r="C15" s="11"/>
@@ -1771,9 +1872,12 @@
       <c r="AA15" s="11"/>
       <c r="AB15" s="3"/>
       <c r="AC15" s="12"/>
-      <c r="AD15" s="12"/>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD15" s="11"/>
+      <c r="AE15" s="3"/>
+      <c r="AF15" s="12"/>
+      <c r="AG15" s="12"/>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A16" s="3"/>
       <c r="B16" s="8"/>
       <c r="C16" s="11"/>
@@ -1803,9 +1907,12 @@
       <c r="AA16" s="11"/>
       <c r="AB16" s="3"/>
       <c r="AC16" s="12"/>
-      <c r="AD16" s="12"/>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD16" s="11"/>
+      <c r="AE16" s="3"/>
+      <c r="AF16" s="12"/>
+      <c r="AG16" s="12"/>
+    </row>
+    <row r="17" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A17" s="3"/>
       <c r="B17" s="8"/>
       <c r="C17" s="11"/>
@@ -1835,9 +1942,12 @@
       <c r="AA17" s="11"/>
       <c r="AB17" s="3"/>
       <c r="AC17" s="12"/>
-      <c r="AD17" s="12"/>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD17" s="11"/>
+      <c r="AE17" s="3"/>
+      <c r="AF17" s="12"/>
+      <c r="AG17" s="12"/>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A18" s="3"/>
       <c r="B18" s="8"/>
       <c r="C18" s="11"/>
@@ -1867,9 +1977,12 @@
       <c r="AA18" s="11"/>
       <c r="AB18" s="3"/>
       <c r="AC18" s="12"/>
-      <c r="AD18" s="12"/>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD18" s="11"/>
+      <c r="AE18" s="3"/>
+      <c r="AF18" s="12"/>
+      <c r="AG18" s="12"/>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A19" s="3"/>
       <c r="B19" s="8"/>
       <c r="C19" s="11"/>
@@ -1899,9 +2012,12 @@
       <c r="AA19" s="11"/>
       <c r="AB19" s="3"/>
       <c r="AC19" s="12"/>
-      <c r="AD19" s="12"/>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD19" s="11"/>
+      <c r="AE19" s="3"/>
+      <c r="AF19" s="12"/>
+      <c r="AG19" s="12"/>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A20" s="3"/>
       <c r="B20" s="8"/>
       <c r="C20" s="11"/>
@@ -1931,9 +2047,12 @@
       <c r="AA20" s="11"/>
       <c r="AB20" s="3"/>
       <c r="AC20" s="12"/>
-      <c r="AD20" s="12"/>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD20" s="11"/>
+      <c r="AE20" s="3"/>
+      <c r="AF20" s="12"/>
+      <c r="AG20" s="12"/>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A21" s="3"/>
       <c r="B21" s="8"/>
       <c r="C21" s="11"/>
@@ -1963,9 +2082,12 @@
       <c r="AA21" s="11"/>
       <c r="AB21" s="3"/>
       <c r="AC21" s="12"/>
-      <c r="AD21" s="12"/>
-    </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD21" s="11"/>
+      <c r="AE21" s="3"/>
+      <c r="AF21" s="12"/>
+      <c r="AG21" s="12"/>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A22" s="3"/>
       <c r="B22" s="8"/>
       <c r="C22" s="11"/>
@@ -1995,9 +2117,12 @@
       <c r="AA22" s="11"/>
       <c r="AB22" s="3"/>
       <c r="AC22" s="12"/>
-      <c r="AD22" s="12"/>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD22" s="11"/>
+      <c r="AE22" s="3"/>
+      <c r="AF22" s="12"/>
+      <c r="AG22" s="12"/>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A23" s="3"/>
       <c r="B23" s="8"/>
       <c r="C23" s="11"/>
@@ -2027,9 +2152,12 @@
       <c r="AA23" s="11"/>
       <c r="AB23" s="3"/>
       <c r="AC23" s="12"/>
-      <c r="AD23" s="12"/>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD23" s="11"/>
+      <c r="AE23" s="3"/>
+      <c r="AF23" s="12"/>
+      <c r="AG23" s="12"/>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A24" s="3"/>
       <c r="B24" s="8"/>
       <c r="C24" s="11"/>
@@ -2059,9 +2187,12 @@
       <c r="AA24" s="11"/>
       <c r="AB24" s="3"/>
       <c r="AC24" s="12"/>
-      <c r="AD24" s="12"/>
-    </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD24" s="11"/>
+      <c r="AE24" s="3"/>
+      <c r="AF24" s="12"/>
+      <c r="AG24" s="12"/>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A25" s="3"/>
       <c r="B25" s="8"/>
       <c r="C25" s="11"/>
@@ -2091,9 +2222,12 @@
       <c r="AA25" s="11"/>
       <c r="AB25" s="3"/>
       <c r="AC25" s="12"/>
-      <c r="AD25" s="12"/>
-    </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD25" s="11"/>
+      <c r="AE25" s="3"/>
+      <c r="AF25" s="12"/>
+      <c r="AG25" s="12"/>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A26" s="3"/>
       <c r="B26" s="8"/>
       <c r="C26" s="11"/>
@@ -2123,9 +2257,12 @@
       <c r="AA26" s="11"/>
       <c r="AB26" s="3"/>
       <c r="AC26" s="12"/>
-      <c r="AD26" s="12"/>
-    </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD26" s="11"/>
+      <c r="AE26" s="3"/>
+      <c r="AF26" s="12"/>
+      <c r="AG26" s="12"/>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A27" s="3"/>
       <c r="B27" s="8"/>
       <c r="C27" s="11"/>
@@ -2155,9 +2292,12 @@
       <c r="AA27" s="11"/>
       <c r="AB27" s="3"/>
       <c r="AC27" s="12"/>
-      <c r="AD27" s="12"/>
-    </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD27" s="11"/>
+      <c r="AE27" s="3"/>
+      <c r="AF27" s="12"/>
+      <c r="AG27" s="12"/>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A28" s="3"/>
       <c r="B28" s="8"/>
       <c r="C28" s="11"/>
@@ -2187,9 +2327,12 @@
       <c r="AA28" s="11"/>
       <c r="AB28" s="3"/>
       <c r="AC28" s="12"/>
-      <c r="AD28" s="12"/>
-    </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD28" s="11"/>
+      <c r="AE28" s="3"/>
+      <c r="AF28" s="12"/>
+      <c r="AG28" s="12"/>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A29" s="3"/>
       <c r="B29" s="8"/>
       <c r="C29" s="11"/>
@@ -2219,9 +2362,12 @@
       <c r="AA29" s="11"/>
       <c r="AB29" s="3"/>
       <c r="AC29" s="12"/>
-      <c r="AD29" s="12"/>
-    </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD29" s="11"/>
+      <c r="AE29" s="3"/>
+      <c r="AF29" s="12"/>
+      <c r="AG29" s="12"/>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A30" s="3"/>
       <c r="B30" s="8"/>
       <c r="C30" s="11"/>
@@ -2251,9 +2397,12 @@
       <c r="AA30" s="11"/>
       <c r="AB30" s="3"/>
       <c r="AC30" s="12"/>
-      <c r="AD30" s="12"/>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD30" s="11"/>
+      <c r="AE30" s="3"/>
+      <c r="AF30" s="12"/>
+      <c r="AG30" s="12"/>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A31" s="3"/>
       <c r="B31" s="8"/>
       <c r="C31" s="11"/>
@@ -2283,9 +2432,12 @@
       <c r="AA31" s="11"/>
       <c r="AB31" s="3"/>
       <c r="AC31" s="12"/>
-      <c r="AD31" s="12"/>
-    </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD31" s="11"/>
+      <c r="AE31" s="3"/>
+      <c r="AF31" s="12"/>
+      <c r="AG31" s="12"/>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A32" s="3"/>
       <c r="B32" s="8"/>
       <c r="C32" s="11"/>
@@ -2315,9 +2467,12 @@
       <c r="AA32" s="11"/>
       <c r="AB32" s="3"/>
       <c r="AC32" s="12"/>
-      <c r="AD32" s="12"/>
-    </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD32" s="11"/>
+      <c r="AE32" s="3"/>
+      <c r="AF32" s="12"/>
+      <c r="AG32" s="12"/>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A33" s="3"/>
       <c r="B33" s="8"/>
       <c r="C33" s="11"/>
@@ -2347,9 +2502,12 @@
       <c r="AA33" s="11"/>
       <c r="AB33" s="3"/>
       <c r="AC33" s="12"/>
-      <c r="AD33" s="12"/>
-    </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD33" s="11"/>
+      <c r="AE33" s="3"/>
+      <c r="AF33" s="12"/>
+      <c r="AG33" s="12"/>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A34" s="3"/>
       <c r="B34" s="8"/>
       <c r="C34" s="11"/>
@@ -2379,9 +2537,12 @@
       <c r="AA34" s="11"/>
       <c r="AB34" s="3"/>
       <c r="AC34" s="12"/>
-      <c r="AD34" s="12"/>
-    </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD34" s="11"/>
+      <c r="AE34" s="3"/>
+      <c r="AF34" s="12"/>
+      <c r="AG34" s="12"/>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A35" s="3"/>
       <c r="B35" s="8"/>
       <c r="C35" s="11"/>
@@ -2411,9 +2572,12 @@
       <c r="AA35" s="11"/>
       <c r="AB35" s="3"/>
       <c r="AC35" s="12"/>
-      <c r="AD35" s="12"/>
-    </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD35" s="11"/>
+      <c r="AE35" s="3"/>
+      <c r="AF35" s="12"/>
+      <c r="AG35" s="12"/>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A36" s="3"/>
       <c r="B36" s="8"/>
       <c r="C36" s="11"/>
@@ -2443,9 +2607,12 @@
       <c r="AA36" s="11"/>
       <c r="AB36" s="3"/>
       <c r="AC36" s="12"/>
-      <c r="AD36" s="12"/>
-    </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD36" s="11"/>
+      <c r="AE36" s="3"/>
+      <c r="AF36" s="12"/>
+      <c r="AG36" s="12"/>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A37" s="3"/>
       <c r="B37" s="8"/>
       <c r="C37" s="11"/>
@@ -2475,9 +2642,12 @@
       <c r="AA37" s="11"/>
       <c r="AB37" s="3"/>
       <c r="AC37" s="12"/>
-      <c r="AD37" s="12"/>
-    </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD37" s="11"/>
+      <c r="AE37" s="3"/>
+      <c r="AF37" s="12"/>
+      <c r="AG37" s="12"/>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A38" s="3"/>
       <c r="B38" s="8"/>
       <c r="C38" s="11"/>
@@ -2507,9 +2677,12 @@
       <c r="AA38" s="11"/>
       <c r="AB38" s="3"/>
       <c r="AC38" s="12"/>
-      <c r="AD38" s="12"/>
-    </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD38" s="11"/>
+      <c r="AE38" s="3"/>
+      <c r="AF38" s="12"/>
+      <c r="AG38" s="12"/>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A39" s="3"/>
       <c r="B39" s="8"/>
       <c r="C39" s="11"/>
@@ -2539,9 +2712,12 @@
       <c r="AA39" s="11"/>
       <c r="AB39" s="3"/>
       <c r="AC39" s="12"/>
-      <c r="AD39" s="12"/>
-    </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD39" s="11"/>
+      <c r="AE39" s="3"/>
+      <c r="AF39" s="12"/>
+      <c r="AG39" s="12"/>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A40" s="3"/>
       <c r="B40" s="8"/>
       <c r="C40" s="11"/>
@@ -2571,9 +2747,12 @@
       <c r="AA40" s="11"/>
       <c r="AB40" s="3"/>
       <c r="AC40" s="12"/>
-      <c r="AD40" s="12"/>
-    </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD40" s="11"/>
+      <c r="AE40" s="3"/>
+      <c r="AF40" s="12"/>
+      <c r="AG40" s="12"/>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A41" s="3"/>
       <c r="B41" s="8"/>
       <c r="C41" s="11"/>
@@ -2603,9 +2782,12 @@
       <c r="AA41" s="11"/>
       <c r="AB41" s="3"/>
       <c r="AC41" s="12"/>
-      <c r="AD41" s="12"/>
-    </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD41" s="11"/>
+      <c r="AE41" s="3"/>
+      <c r="AF41" s="12"/>
+      <c r="AG41" s="12"/>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A42" s="3"/>
       <c r="B42" s="8"/>
       <c r="C42" s="11"/>
@@ -2635,9 +2817,12 @@
       <c r="AA42" s="11"/>
       <c r="AB42" s="3"/>
       <c r="AC42" s="12"/>
-      <c r="AD42" s="12"/>
-    </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD42" s="11"/>
+      <c r="AE42" s="3"/>
+      <c r="AF42" s="12"/>
+      <c r="AG42" s="12"/>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A43" s="3"/>
       <c r="B43" s="8"/>
       <c r="C43" s="11"/>
@@ -2667,9 +2852,12 @@
       <c r="AA43" s="11"/>
       <c r="AB43" s="3"/>
       <c r="AC43" s="12"/>
-      <c r="AD43" s="12"/>
-    </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD43" s="11"/>
+      <c r="AE43" s="3"/>
+      <c r="AF43" s="12"/>
+      <c r="AG43" s="12"/>
+    </row>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A44" s="3"/>
       <c r="B44" s="8"/>
       <c r="C44" s="11"/>
@@ -2699,9 +2887,12 @@
       <c r="AA44" s="11"/>
       <c r="AB44" s="3"/>
       <c r="AC44" s="12"/>
-      <c r="AD44" s="12"/>
-    </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD44" s="11"/>
+      <c r="AE44" s="3"/>
+      <c r="AF44" s="12"/>
+      <c r="AG44" s="12"/>
+    </row>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A45" s="3"/>
       <c r="B45" s="8"/>
       <c r="C45" s="11"/>
@@ -2731,9 +2922,12 @@
       <c r="AA45" s="11"/>
       <c r="AB45" s="3"/>
       <c r="AC45" s="12"/>
-      <c r="AD45" s="12"/>
-    </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD45" s="11"/>
+      <c r="AE45" s="3"/>
+      <c r="AF45" s="12"/>
+      <c r="AG45" s="12"/>
+    </row>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A46" s="3"/>
       <c r="B46" s="8"/>
       <c r="C46" s="11"/>
@@ -2763,9 +2957,12 @@
       <c r="AA46" s="11"/>
       <c r="AB46" s="3"/>
       <c r="AC46" s="12"/>
-      <c r="AD46" s="12"/>
-    </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD46" s="11"/>
+      <c r="AE46" s="3"/>
+      <c r="AF46" s="12"/>
+      <c r="AG46" s="12"/>
+    </row>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A47" s="3"/>
       <c r="B47" s="8"/>
       <c r="C47" s="11"/>
@@ -2795,9 +2992,12 @@
       <c r="AA47" s="11"/>
       <c r="AB47" s="3"/>
       <c r="AC47" s="12"/>
-      <c r="AD47" s="12"/>
-    </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD47" s="11"/>
+      <c r="AE47" s="3"/>
+      <c r="AF47" s="12"/>
+      <c r="AG47" s="12"/>
+    </row>
+    <row r="48" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A48" s="3"/>
       <c r="B48" s="8"/>
       <c r="C48" s="11"/>
@@ -2827,9 +3027,12 @@
       <c r="AA48" s="11"/>
       <c r="AB48" s="3"/>
       <c r="AC48" s="12"/>
-      <c r="AD48" s="12"/>
-    </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD48" s="11"/>
+      <c r="AE48" s="3"/>
+      <c r="AF48" s="12"/>
+      <c r="AG48" s="12"/>
+    </row>
+    <row r="49" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A49" s="3"/>
       <c r="B49" s="8"/>
       <c r="C49" s="11"/>
@@ -2859,9 +3062,12 @@
       <c r="AA49" s="11"/>
       <c r="AB49" s="3"/>
       <c r="AC49" s="12"/>
-      <c r="AD49" s="12"/>
-    </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD49" s="11"/>
+      <c r="AE49" s="3"/>
+      <c r="AF49" s="12"/>
+      <c r="AG49" s="12"/>
+    </row>
+    <row r="50" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A50" s="3"/>
       <c r="B50" s="8"/>
       <c r="C50" s="11"/>
@@ -2891,9 +3097,12 @@
       <c r="AA50" s="11"/>
       <c r="AB50" s="3"/>
       <c r="AC50" s="12"/>
-      <c r="AD50" s="12"/>
-    </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD50" s="11"/>
+      <c r="AE50" s="3"/>
+      <c r="AF50" s="12"/>
+      <c r="AG50" s="12"/>
+    </row>
+    <row r="51" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A51" s="3"/>
       <c r="B51" s="8"/>
       <c r="C51" s="11"/>
@@ -2923,9 +3132,12 @@
       <c r="AA51" s="11"/>
       <c r="AB51" s="3"/>
       <c r="AC51" s="12"/>
-      <c r="AD51" s="12"/>
-    </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD51" s="11"/>
+      <c r="AE51" s="3"/>
+      <c r="AF51" s="12"/>
+      <c r="AG51" s="12"/>
+    </row>
+    <row r="52" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A52" s="3"/>
       <c r="B52" s="8"/>
       <c r="C52" s="11"/>
@@ -2955,9 +3167,12 @@
       <c r="AA52" s="11"/>
       <c r="AB52" s="3"/>
       <c r="AC52" s="12"/>
-      <c r="AD52" s="12"/>
-    </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD52" s="11"/>
+      <c r="AE52" s="3"/>
+      <c r="AF52" s="12"/>
+      <c r="AG52" s="12"/>
+    </row>
+    <row r="53" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A53" s="3"/>
       <c r="B53" s="8"/>
       <c r="C53" s="11"/>
@@ -2987,9 +3202,12 @@
       <c r="AA53" s="11"/>
       <c r="AB53" s="3"/>
       <c r="AC53" s="12"/>
-      <c r="AD53" s="12"/>
-    </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD53" s="11"/>
+      <c r="AE53" s="3"/>
+      <c r="AF53" s="12"/>
+      <c r="AG53" s="12"/>
+    </row>
+    <row r="54" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A54" s="3"/>
       <c r="B54" s="8"/>
       <c r="C54" s="11"/>
@@ -3019,9 +3237,12 @@
       <c r="AA54" s="11"/>
       <c r="AB54" s="3"/>
       <c r="AC54" s="12"/>
-      <c r="AD54" s="12"/>
-    </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD54" s="11"/>
+      <c r="AE54" s="3"/>
+      <c r="AF54" s="12"/>
+      <c r="AG54" s="12"/>
+    </row>
+    <row r="55" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A55" s="3"/>
       <c r="B55" s="8"/>
       <c r="C55" s="11"/>
@@ -3051,9 +3272,12 @@
       <c r="AA55" s="11"/>
       <c r="AB55" s="3"/>
       <c r="AC55" s="12"/>
-      <c r="AD55" s="12"/>
-    </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD55" s="11"/>
+      <c r="AE55" s="3"/>
+      <c r="AF55" s="12"/>
+      <c r="AG55" s="12"/>
+    </row>
+    <row r="56" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A56" s="3"/>
       <c r="B56" s="8"/>
       <c r="C56" s="11"/>
@@ -3083,9 +3307,12 @@
       <c r="AA56" s="11"/>
       <c r="AB56" s="3"/>
       <c r="AC56" s="12"/>
-      <c r="AD56" s="12"/>
-    </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD56" s="11"/>
+      <c r="AE56" s="3"/>
+      <c r="AF56" s="12"/>
+      <c r="AG56" s="12"/>
+    </row>
+    <row r="57" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A57" s="3"/>
       <c r="B57" s="8"/>
       <c r="C57" s="11"/>
@@ -3115,9 +3342,12 @@
       <c r="AA57" s="11"/>
       <c r="AB57" s="3"/>
       <c r="AC57" s="12"/>
-      <c r="AD57" s="12"/>
-    </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD57" s="11"/>
+      <c r="AE57" s="3"/>
+      <c r="AF57" s="12"/>
+      <c r="AG57" s="12"/>
+    </row>
+    <row r="58" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A58" s="3"/>
       <c r="B58" s="8"/>
       <c r="C58" s="11"/>
@@ -3147,9 +3377,12 @@
       <c r="AA58" s="11"/>
       <c r="AB58" s="3"/>
       <c r="AC58" s="12"/>
-      <c r="AD58" s="12"/>
-    </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD58" s="11"/>
+      <c r="AE58" s="3"/>
+      <c r="AF58" s="12"/>
+      <c r="AG58" s="12"/>
+    </row>
+    <row r="59" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A59" s="3"/>
       <c r="B59" s="8"/>
       <c r="C59" s="11"/>
@@ -3179,9 +3412,12 @@
       <c r="AA59" s="11"/>
       <c r="AB59" s="3"/>
       <c r="AC59" s="12"/>
-      <c r="AD59" s="12"/>
-    </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD59" s="11"/>
+      <c r="AE59" s="3"/>
+      <c r="AF59" s="12"/>
+      <c r="AG59" s="12"/>
+    </row>
+    <row r="60" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A60" s="3"/>
       <c r="B60" s="8"/>
       <c r="C60" s="11"/>
@@ -3211,9 +3447,12 @@
       <c r="AA60" s="11"/>
       <c r="AB60" s="3"/>
       <c r="AC60" s="12"/>
-      <c r="AD60" s="12"/>
-    </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD60" s="11"/>
+      <c r="AE60" s="3"/>
+      <c r="AF60" s="12"/>
+      <c r="AG60" s="12"/>
+    </row>
+    <row r="61" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A61" s="3"/>
       <c r="B61" s="8"/>
       <c r="C61" s="11"/>
@@ -3243,9 +3482,12 @@
       <c r="AA61" s="11"/>
       <c r="AB61" s="3"/>
       <c r="AC61" s="12"/>
-      <c r="AD61" s="12"/>
-    </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD61" s="11"/>
+      <c r="AE61" s="3"/>
+      <c r="AF61" s="12"/>
+      <c r="AG61" s="12"/>
+    </row>
+    <row r="62" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A62" s="3"/>
       <c r="B62" s="8"/>
       <c r="C62" s="11"/>
@@ -3275,9 +3517,12 @@
       <c r="AA62" s="11"/>
       <c r="AB62" s="3"/>
       <c r="AC62" s="12"/>
-      <c r="AD62" s="12"/>
-    </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD62" s="11"/>
+      <c r="AE62" s="3"/>
+      <c r="AF62" s="12"/>
+      <c r="AG62" s="12"/>
+    </row>
+    <row r="63" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A63" s="3"/>
       <c r="B63" s="8"/>
       <c r="C63" s="11"/>
@@ -3307,9 +3552,12 @@
       <c r="AA63" s="11"/>
       <c r="AB63" s="3"/>
       <c r="AC63" s="12"/>
-      <c r="AD63" s="12"/>
-    </row>
-    <row r="64" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD63" s="11"/>
+      <c r="AE63" s="3"/>
+      <c r="AF63" s="12"/>
+      <c r="AG63" s="12"/>
+    </row>
+    <row r="64" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A64" s="3"/>
       <c r="B64" s="8"/>
       <c r="C64" s="11"/>
@@ -3339,9 +3587,12 @@
       <c r="AA64" s="11"/>
       <c r="AB64" s="3"/>
       <c r="AC64" s="12"/>
-      <c r="AD64" s="12"/>
-    </row>
-    <row r="65" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD64" s="11"/>
+      <c r="AE64" s="3"/>
+      <c r="AF64" s="12"/>
+      <c r="AG64" s="12"/>
+    </row>
+    <row r="65" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A65" s="3"/>
       <c r="B65" s="8"/>
       <c r="C65" s="11"/>
@@ -3371,9 +3622,12 @@
       <c r="AA65" s="11"/>
       <c r="AB65" s="3"/>
       <c r="AC65" s="12"/>
-      <c r="AD65" s="12"/>
-    </row>
-    <row r="66" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD65" s="11"/>
+      <c r="AE65" s="3"/>
+      <c r="AF65" s="12"/>
+      <c r="AG65" s="12"/>
+    </row>
+    <row r="66" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A66" s="3"/>
       <c r="B66" s="8"/>
       <c r="C66" s="11"/>
@@ -3403,9 +3657,12 @@
       <c r="AA66" s="11"/>
       <c r="AB66" s="3"/>
       <c r="AC66" s="12"/>
-      <c r="AD66" s="12"/>
-    </row>
-    <row r="67" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD66" s="11"/>
+      <c r="AE66" s="3"/>
+      <c r="AF66" s="12"/>
+      <c r="AG66" s="12"/>
+    </row>
+    <row r="67" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A67" s="3"/>
       <c r="B67" s="8"/>
       <c r="C67" s="11"/>
@@ -3435,9 +3692,12 @@
       <c r="AA67" s="11"/>
       <c r="AB67" s="3"/>
       <c r="AC67" s="12"/>
-      <c r="AD67" s="12"/>
-    </row>
-    <row r="68" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD67" s="11"/>
+      <c r="AE67" s="3"/>
+      <c r="AF67" s="12"/>
+      <c r="AG67" s="12"/>
+    </row>
+    <row r="68" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A68" s="3"/>
       <c r="B68" s="8"/>
       <c r="C68" s="11"/>
@@ -3467,9 +3727,12 @@
       <c r="AA68" s="11"/>
       <c r="AB68" s="3"/>
       <c r="AC68" s="12"/>
-      <c r="AD68" s="12"/>
-    </row>
-    <row r="69" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD68" s="11"/>
+      <c r="AE68" s="3"/>
+      <c r="AF68" s="12"/>
+      <c r="AG68" s="12"/>
+    </row>
+    <row r="69" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A69" s="3"/>
       <c r="B69" s="8"/>
       <c r="C69" s="11"/>
@@ -3499,9 +3762,12 @@
       <c r="AA69" s="11"/>
       <c r="AB69" s="3"/>
       <c r="AC69" s="12"/>
-      <c r="AD69" s="12"/>
-    </row>
-    <row r="70" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD69" s="11"/>
+      <c r="AE69" s="3"/>
+      <c r="AF69" s="12"/>
+      <c r="AG69" s="12"/>
+    </row>
+    <row r="70" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A70" s="3"/>
       <c r="B70" s="8"/>
       <c r="C70" s="11"/>
@@ -3531,9 +3797,12 @@
       <c r="AA70" s="11"/>
       <c r="AB70" s="3"/>
       <c r="AC70" s="12"/>
-      <c r="AD70" s="12"/>
-    </row>
-    <row r="71" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD70" s="11"/>
+      <c r="AE70" s="3"/>
+      <c r="AF70" s="12"/>
+      <c r="AG70" s="12"/>
+    </row>
+    <row r="71" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A71" s="3"/>
       <c r="B71" s="8"/>
       <c r="C71" s="11"/>
@@ -3563,9 +3832,12 @@
       <c r="AA71" s="11"/>
       <c r="AB71" s="3"/>
       <c r="AC71" s="12"/>
-      <c r="AD71" s="12"/>
-    </row>
-    <row r="72" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD71" s="11"/>
+      <c r="AE71" s="3"/>
+      <c r="AF71" s="12"/>
+      <c r="AG71" s="12"/>
+    </row>
+    <row r="72" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A72" s="3"/>
       <c r="B72" s="8"/>
       <c r="C72" s="11"/>
@@ -3595,9 +3867,12 @@
       <c r="AA72" s="11"/>
       <c r="AB72" s="3"/>
       <c r="AC72" s="12"/>
-      <c r="AD72" s="12"/>
-    </row>
-    <row r="73" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD72" s="11"/>
+      <c r="AE72" s="3"/>
+      <c r="AF72" s="12"/>
+      <c r="AG72" s="12"/>
+    </row>
+    <row r="73" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A73" s="3"/>
       <c r="B73" s="8"/>
       <c r="C73" s="11"/>
@@ -3627,9 +3902,12 @@
       <c r="AA73" s="11"/>
       <c r="AB73" s="3"/>
       <c r="AC73" s="12"/>
-      <c r="AD73" s="12"/>
-    </row>
-    <row r="74" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD73" s="11"/>
+      <c r="AE73" s="3"/>
+      <c r="AF73" s="12"/>
+      <c r="AG73" s="12"/>
+    </row>
+    <row r="74" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A74" s="3"/>
       <c r="B74" s="8"/>
       <c r="C74" s="11"/>
@@ -3659,9 +3937,12 @@
       <c r="AA74" s="11"/>
       <c r="AB74" s="3"/>
       <c r="AC74" s="12"/>
-      <c r="AD74" s="12"/>
-    </row>
-    <row r="75" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD74" s="11"/>
+      <c r="AE74" s="3"/>
+      <c r="AF74" s="12"/>
+      <c r="AG74" s="12"/>
+    </row>
+    <row r="75" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A75" s="3"/>
       <c r="B75" s="8"/>
       <c r="C75" s="11"/>
@@ -3691,9 +3972,12 @@
       <c r="AA75" s="11"/>
       <c r="AB75" s="3"/>
       <c r="AC75" s="12"/>
-      <c r="AD75" s="12"/>
-    </row>
-    <row r="76" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD75" s="11"/>
+      <c r="AE75" s="3"/>
+      <c r="AF75" s="12"/>
+      <c r="AG75" s="12"/>
+    </row>
+    <row r="76" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A76" s="3"/>
       <c r="B76" s="8"/>
       <c r="C76" s="11"/>
@@ -3723,9 +4007,12 @@
       <c r="AA76" s="11"/>
       <c r="AB76" s="3"/>
       <c r="AC76" s="12"/>
-      <c r="AD76" s="12"/>
-    </row>
-    <row r="77" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD76" s="11"/>
+      <c r="AE76" s="3"/>
+      <c r="AF76" s="12"/>
+      <c r="AG76" s="12"/>
+    </row>
+    <row r="77" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A77" s="3"/>
       <c r="B77" s="8"/>
       <c r="C77" s="11"/>
@@ -3755,9 +4042,12 @@
       <c r="AA77" s="11"/>
       <c r="AB77" s="3"/>
       <c r="AC77" s="12"/>
-      <c r="AD77" s="12"/>
-    </row>
-    <row r="78" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD77" s="11"/>
+      <c r="AE77" s="3"/>
+      <c r="AF77" s="12"/>
+      <c r="AG77" s="12"/>
+    </row>
+    <row r="78" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A78" s="3"/>
       <c r="B78" s="8"/>
       <c r="C78" s="11"/>
@@ -3787,9 +4077,12 @@
       <c r="AA78" s="11"/>
       <c r="AB78" s="3"/>
       <c r="AC78" s="12"/>
-      <c r="AD78" s="12"/>
-    </row>
-    <row r="79" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD78" s="11"/>
+      <c r="AE78" s="3"/>
+      <c r="AF78" s="12"/>
+      <c r="AG78" s="12"/>
+    </row>
+    <row r="79" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A79" s="3"/>
       <c r="B79" s="8"/>
       <c r="C79" s="11"/>
@@ -3819,9 +4112,12 @@
       <c r="AA79" s="11"/>
       <c r="AB79" s="3"/>
       <c r="AC79" s="12"/>
-      <c r="AD79" s="12"/>
-    </row>
-    <row r="80" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD79" s="11"/>
+      <c r="AE79" s="3"/>
+      <c r="AF79" s="12"/>
+      <c r="AG79" s="12"/>
+    </row>
+    <row r="80" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A80" s="3"/>
       <c r="B80" s="8"/>
       <c r="C80" s="11"/>
@@ -3851,9 +4147,12 @@
       <c r="AA80" s="11"/>
       <c r="AB80" s="3"/>
       <c r="AC80" s="12"/>
-      <c r="AD80" s="12"/>
-    </row>
-    <row r="81" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD80" s="11"/>
+      <c r="AE80" s="3"/>
+      <c r="AF80" s="12"/>
+      <c r="AG80" s="12"/>
+    </row>
+    <row r="81" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A81" s="3"/>
       <c r="B81" s="8"/>
       <c r="C81" s="11"/>
@@ -3883,9 +4182,12 @@
       <c r="AA81" s="11"/>
       <c r="AB81" s="3"/>
       <c r="AC81" s="12"/>
-      <c r="AD81" s="12"/>
-    </row>
-    <row r="82" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD81" s="11"/>
+      <c r="AE81" s="3"/>
+      <c r="AF81" s="12"/>
+      <c r="AG81" s="12"/>
+    </row>
+    <row r="82" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A82" s="3"/>
       <c r="B82" s="8"/>
       <c r="C82" s="11"/>
@@ -3915,9 +4217,12 @@
       <c r="AA82" s="11"/>
       <c r="AB82" s="3"/>
       <c r="AC82" s="12"/>
-      <c r="AD82" s="12"/>
-    </row>
-    <row r="83" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD82" s="11"/>
+      <c r="AE82" s="3"/>
+      <c r="AF82" s="12"/>
+      <c r="AG82" s="12"/>
+    </row>
+    <row r="83" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A83" s="3"/>
       <c r="B83" s="8"/>
       <c r="C83" s="11"/>
@@ -3947,9 +4252,12 @@
       <c r="AA83" s="11"/>
       <c r="AB83" s="3"/>
       <c r="AC83" s="12"/>
-      <c r="AD83" s="12"/>
-    </row>
-    <row r="84" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD83" s="11"/>
+      <c r="AE83" s="3"/>
+      <c r="AF83" s="12"/>
+      <c r="AG83" s="12"/>
+    </row>
+    <row r="84" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A84" s="3"/>
       <c r="B84" s="8"/>
       <c r="C84" s="11"/>
@@ -3979,9 +4287,12 @@
       <c r="AA84" s="11"/>
       <c r="AB84" s="3"/>
       <c r="AC84" s="12"/>
-      <c r="AD84" s="12"/>
-    </row>
-    <row r="85" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD84" s="11"/>
+      <c r="AE84" s="3"/>
+      <c r="AF84" s="12"/>
+      <c r="AG84" s="12"/>
+    </row>
+    <row r="85" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A85" s="3"/>
       <c r="B85" s="8"/>
       <c r="C85" s="11"/>
@@ -4011,9 +4322,12 @@
       <c r="AA85" s="11"/>
       <c r="AB85" s="3"/>
       <c r="AC85" s="12"/>
-      <c r="AD85" s="12"/>
-    </row>
-    <row r="86" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD85" s="11"/>
+      <c r="AE85" s="3"/>
+      <c r="AF85" s="12"/>
+      <c r="AG85" s="12"/>
+    </row>
+    <row r="86" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A86" s="3"/>
       <c r="B86" s="8"/>
       <c r="C86" s="11"/>
@@ -4043,9 +4357,12 @@
       <c r="AA86" s="11"/>
       <c r="AB86" s="3"/>
       <c r="AC86" s="12"/>
-      <c r="AD86" s="12"/>
-    </row>
-    <row r="87" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD86" s="11"/>
+      <c r="AE86" s="3"/>
+      <c r="AF86" s="12"/>
+      <c r="AG86" s="12"/>
+    </row>
+    <row r="87" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A87" s="3"/>
       <c r="B87" s="8"/>
       <c r="C87" s="11"/>
@@ -4075,9 +4392,12 @@
       <c r="AA87" s="11"/>
       <c r="AB87" s="3"/>
       <c r="AC87" s="12"/>
-      <c r="AD87" s="12"/>
-    </row>
-    <row r="88" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD87" s="11"/>
+      <c r="AE87" s="3"/>
+      <c r="AF87" s="12"/>
+      <c r="AG87" s="12"/>
+    </row>
+    <row r="88" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A88" s="3"/>
       <c r="B88" s="8"/>
       <c r="C88" s="11"/>
@@ -4107,9 +4427,12 @@
       <c r="AA88" s="11"/>
       <c r="AB88" s="3"/>
       <c r="AC88" s="12"/>
-      <c r="AD88" s="12"/>
-    </row>
-    <row r="89" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD88" s="11"/>
+      <c r="AE88" s="3"/>
+      <c r="AF88" s="12"/>
+      <c r="AG88" s="12"/>
+    </row>
+    <row r="89" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A89" s="3"/>
       <c r="B89" s="8"/>
       <c r="C89" s="11"/>
@@ -4139,9 +4462,12 @@
       <c r="AA89" s="11"/>
       <c r="AB89" s="3"/>
       <c r="AC89" s="12"/>
-      <c r="AD89" s="12"/>
-    </row>
-    <row r="90" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD89" s="11"/>
+      <c r="AE89" s="3"/>
+      <c r="AF89" s="12"/>
+      <c r="AG89" s="12"/>
+    </row>
+    <row r="90" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A90" s="3"/>
       <c r="B90" s="8"/>
       <c r="C90" s="11"/>
@@ -4171,9 +4497,12 @@
       <c r="AA90" s="11"/>
       <c r="AB90" s="3"/>
       <c r="AC90" s="12"/>
-      <c r="AD90" s="12"/>
-    </row>
-    <row r="91" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD90" s="11"/>
+      <c r="AE90" s="3"/>
+      <c r="AF90" s="12"/>
+      <c r="AG90" s="12"/>
+    </row>
+    <row r="91" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A91" s="3"/>
       <c r="B91" s="8"/>
       <c r="C91" s="11"/>
@@ -4203,9 +4532,12 @@
       <c r="AA91" s="11"/>
       <c r="AB91" s="3"/>
       <c r="AC91" s="12"/>
-      <c r="AD91" s="12"/>
-    </row>
-    <row r="92" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD91" s="11"/>
+      <c r="AE91" s="3"/>
+      <c r="AF91" s="12"/>
+      <c r="AG91" s="12"/>
+    </row>
+    <row r="92" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A92" s="3"/>
       <c r="B92" s="8"/>
       <c r="C92" s="11"/>
@@ -4235,9 +4567,12 @@
       <c r="AA92" s="11"/>
       <c r="AB92" s="3"/>
       <c r="AC92" s="12"/>
-      <c r="AD92" s="12"/>
-    </row>
-    <row r="93" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD92" s="11"/>
+      <c r="AE92" s="3"/>
+      <c r="AF92" s="12"/>
+      <c r="AG92" s="12"/>
+    </row>
+    <row r="93" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A93" s="3"/>
       <c r="B93" s="8"/>
       <c r="C93" s="11"/>
@@ -4267,9 +4602,12 @@
       <c r="AA93" s="11"/>
       <c r="AB93" s="3"/>
       <c r="AC93" s="12"/>
-      <c r="AD93" s="12"/>
-    </row>
-    <row r="94" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD93" s="11"/>
+      <c r="AE93" s="3"/>
+      <c r="AF93" s="12"/>
+      <c r="AG93" s="12"/>
+    </row>
+    <row r="94" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A94" s="3"/>
       <c r="B94" s="8"/>
       <c r="C94" s="11"/>
@@ -4299,9 +4637,12 @@
       <c r="AA94" s="11"/>
       <c r="AB94" s="3"/>
       <c r="AC94" s="12"/>
-      <c r="AD94" s="12"/>
-    </row>
-    <row r="95" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD94" s="11"/>
+      <c r="AE94" s="3"/>
+      <c r="AF94" s="12"/>
+      <c r="AG94" s="12"/>
+    </row>
+    <row r="95" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A95" s="3"/>
       <c r="B95" s="8"/>
       <c r="C95" s="11"/>
@@ -4331,9 +4672,12 @@
       <c r="AA95" s="11"/>
       <c r="AB95" s="3"/>
       <c r="AC95" s="12"/>
-      <c r="AD95" s="12"/>
-    </row>
-    <row r="96" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD95" s="11"/>
+      <c r="AE95" s="3"/>
+      <c r="AF95" s="12"/>
+      <c r="AG95" s="12"/>
+    </row>
+    <row r="96" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A96" s="3"/>
       <c r="B96" s="8"/>
       <c r="C96" s="11"/>
@@ -4363,9 +4707,12 @@
       <c r="AA96" s="11"/>
       <c r="AB96" s="3"/>
       <c r="AC96" s="12"/>
-      <c r="AD96" s="12"/>
-    </row>
-    <row r="97" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD96" s="11"/>
+      <c r="AE96" s="3"/>
+      <c r="AF96" s="12"/>
+      <c r="AG96" s="12"/>
+    </row>
+    <row r="97" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A97" s="3"/>
       <c r="B97" s="8"/>
       <c r="C97" s="11"/>
@@ -4395,9 +4742,12 @@
       <c r="AA97" s="11"/>
       <c r="AB97" s="3"/>
       <c r="AC97" s="12"/>
-      <c r="AD97" s="12"/>
-    </row>
-    <row r="98" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD97" s="11"/>
+      <c r="AE97" s="3"/>
+      <c r="AF97" s="12"/>
+      <c r="AG97" s="12"/>
+    </row>
+    <row r="98" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A98" s="3"/>
       <c r="B98" s="8"/>
       <c r="C98" s="11"/>
@@ -4427,9 +4777,12 @@
       <c r="AA98" s="11"/>
       <c r="AB98" s="3"/>
       <c r="AC98" s="12"/>
-      <c r="AD98" s="12"/>
-    </row>
-    <row r="99" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD98" s="11"/>
+      <c r="AE98" s="3"/>
+      <c r="AF98" s="12"/>
+      <c r="AG98" s="12"/>
+    </row>
+    <row r="99" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A99" s="3"/>
       <c r="B99" s="8"/>
       <c r="C99" s="11"/>
@@ -4459,9 +4812,12 @@
       <c r="AA99" s="11"/>
       <c r="AB99" s="3"/>
       <c r="AC99" s="12"/>
-      <c r="AD99" s="12"/>
-    </row>
-    <row r="100" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD99" s="11"/>
+      <c r="AE99" s="3"/>
+      <c r="AF99" s="12"/>
+      <c r="AG99" s="12"/>
+    </row>
+    <row r="100" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A100" s="3"/>
       <c r="B100" s="8"/>
       <c r="C100" s="11"/>
@@ -4491,9 +4847,12 @@
       <c r="AA100" s="11"/>
       <c r="AB100" s="3"/>
       <c r="AC100" s="12"/>
-      <c r="AD100" s="12"/>
-    </row>
-    <row r="101" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD100" s="11"/>
+      <c r="AE100" s="3"/>
+      <c r="AF100" s="12"/>
+      <c r="AG100" s="12"/>
+    </row>
+    <row r="101" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A101" s="3"/>
       <c r="B101" s="8"/>
       <c r="C101" s="11"/>
@@ -4523,9 +4882,12 @@
       <c r="AA101" s="11"/>
       <c r="AB101" s="3"/>
       <c r="AC101" s="12"/>
-      <c r="AD101" s="12"/>
-    </row>
-    <row r="102" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD101" s="11"/>
+      <c r="AE101" s="3"/>
+      <c r="AF101" s="12"/>
+      <c r="AG101" s="12"/>
+    </row>
+    <row r="102" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A102" s="3"/>
       <c r="B102" s="8"/>
       <c r="C102" s="11"/>
@@ -4555,9 +4917,12 @@
       <c r="AA102" s="11"/>
       <c r="AB102" s="3"/>
       <c r="AC102" s="12"/>
-      <c r="AD102" s="12"/>
-    </row>
-    <row r="103" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD102" s="11"/>
+      <c r="AE102" s="3"/>
+      <c r="AF102" s="12"/>
+      <c r="AG102" s="12"/>
+    </row>
+    <row r="103" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A103" s="35"/>
       <c r="B103" s="36"/>
       <c r="C103" s="37"/>
@@ -4587,9 +4952,12 @@
       <c r="AA103" s="37"/>
       <c r="AB103" s="35"/>
       <c r="AC103" s="38"/>
-      <c r="AD103" s="38"/>
-    </row>
-    <row r="104" spans="1:30" x14ac:dyDescent="0.4">
+      <c r="AD103" s="37"/>
+      <c r="AE103" s="35"/>
+      <c r="AF103" s="38"/>
+      <c r="AG103" s="38"/>
+    </row>
+    <row r="104" spans="1:33" x14ac:dyDescent="0.4">
       <c r="A104" s="39"/>
       <c r="B104" s="39"/>
       <c r="C104" s="39"/>
@@ -4620,6 +4988,9 @@
       <c r="AB104" s="39"/>
       <c r="AC104" s="39"/>
       <c r="AD104" s="39"/>
+      <c r="AE104" s="39"/>
+      <c r="AF104" s="39"/>
+      <c r="AG104" s="39"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
fix: [gm_scene_play.cpp/h]  nullptr reference.
</commit_message>
<xml_diff>
--- a/CoordinateData_Robot1_01.xlsx
+++ b/CoordinateData_Robot1_01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waltz\Documents\CppProjects\GitManagements\QuantumCoreRobotReNew_0104\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C87FB26B-325F-46B9-BA4D-E21E676A5DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{27512861-E88E-453C-A638-572E1597667E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="2280" windowWidth="29040" windowHeight="15840" xr2:uid="{4A88D659-4C13-44B6-A2BE-41980A9F7671}"/>
   </bookViews>
@@ -991,7 +991,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:AD4"/>
+      <selection pane="bottomLeft" activeCell="AF7" sqref="AF7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1291,7 +1291,7 @@
         <v>28</v>
       </c>
       <c r="AE4" s="4">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="AF4" s="28">
         <v>0.5</v>
@@ -1390,7 +1390,7 @@
         <v>28</v>
       </c>
       <c r="AE5" s="4">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="AF5" s="28">
         <v>0.5</v>
@@ -1489,7 +1489,7 @@
         <v>28</v>
       </c>
       <c r="AE6" s="4">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="AF6" s="28">
         <v>0.5</v>
@@ -1588,7 +1588,7 @@
         <v>28</v>
       </c>
       <c r="AE7" s="4">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="AF7" s="28">
         <v>0.5</v>

</xml_diff>